<commit_message>
Refactor : 엑셀 예시 파일 수정 (#15)
</commit_message>
<xml_diff>
--- a/src/main/resources/static/excel/example.xlsx
+++ b/src/main/resources/static/excel/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeongchanmin/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F775AD67-B250-7540-8B8A-8E10D76D692B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B040E509-9CE3-9B42-B0B6-C7B99674DE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17120" activeTab="2" xr2:uid="{B0100E95-B2E1-0041-8469-1265C212210E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="126">
   <si>
     <t>name</t>
   </si>
@@ -52,118 +52,16 @@
     <t>answer</t>
   </si>
   <si>
-    <t>wrong_answer</t>
-  </si>
-  <si>
     <t>OX</t>
   </si>
   <si>
-    <t>Is an apple a fruit?</t>
-  </si>
-  <si>
     <t>O</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>An apple is a fruit, typically red or green.</t>
-  </si>
-  <si>
     <t>MULTIPLE_CHOICE_SHORT</t>
   </si>
   <si>
-    <t>What is a table?</t>
-  </si>
-  <si>
-    <t>Furniture</t>
-  </si>
-  <si>
-    <t>Animal</t>
-  </si>
-  <si>
-    <t>A table is a piece of furniture with a flat surface.</t>
-  </si>
-  <si>
     <t>MULTIPLE_CHOICE_LONG</t>
-  </si>
-  <si>
-    <t>What is an elephant?</t>
-  </si>
-  <si>
-    <t>A large animal</t>
-  </si>
-  <si>
-    <t>A bird</t>
-  </si>
-  <si>
-    <t>An elephant is a large mammal with a trunk.</t>
-  </si>
-  <si>
-    <t>Is Python a programming language?</t>
-  </si>
-  <si>
-    <t>Python is a high-level programming language.</t>
-  </si>
-  <si>
-    <t>What is a mountain?</t>
-  </si>
-  <si>
-    <t>A landform</t>
-  </si>
-  <si>
-    <t>A river</t>
-  </si>
-  <si>
-    <t>A mountain is a large landform that rises above the surrounding land.</t>
-  </si>
-  <si>
-    <t>What is a car?</t>
-  </si>
-  <si>
-    <t>A vehicle</t>
-  </si>
-  <si>
-    <t>A building</t>
-  </si>
-  <si>
-    <t>A car is a vehicle used for transportation.</t>
-  </si>
-  <si>
-    <t>Is a guitar a musical instrument?</t>
-  </si>
-  <si>
-    <t>A guitar is a musical instrument with strings.</t>
-  </si>
-  <si>
-    <t>What is a sunflower?</t>
-  </si>
-  <si>
-    <t>A flower</t>
-  </si>
-  <si>
-    <t>A tree</t>
-  </si>
-  <si>
-    <t>A sunflower is a tall, bright yellow flower.</t>
-  </si>
-  <si>
-    <t>What is an ocean?</t>
-  </si>
-  <si>
-    <t>A large body of water</t>
-  </si>
-  <si>
-    <t>A forest</t>
-  </si>
-  <si>
-    <t>An ocean is a large body of saltwater.</t>
-  </si>
-  <si>
-    <t>Is a computer an electronic device?</t>
-  </si>
-  <si>
-    <t>A computer is an electronic device used for processing information.</t>
   </si>
   <si>
     <t>기본 경제 개념</t>
@@ -888,12 +786,859 @@
   <si>
     <t>예금과 대출</t>
   </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>choices</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>수요가 증가하면 일반적으로 상품의 가격이 상승하는 경향이 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>수요 곡선과 공급 곡선이 교차하는 지점에서 결정되는 가격은 무엇인가요?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">수요가 증가하면 상품을 사고 싶어 하는 사람이 많아져요. 이때 공급량이 일정하다면 상품의 가격이 올라요. 예를 들어, 여름철 더위로 아이스크림을 찾는 사람이 많아지면 아이스크림의 가격이 오를 가능성이 커요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 수요가 증가하면 가격이 상승하는 경향이 있어요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>균형 가격</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">수요 곡선과 공급 곡선은 시장에서 상품의 가격과 거래량을 결정하는 데 중요한 역할을 해요. 이 두 곡선이 교차하는 지점이 바로 **균형 가격**이에요. 균형 가격에서는 소비자가 사고 싶어 하는 양과 생산자가 팔고 싶어 하는 양이 일치해요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 균형 가격은 시장의 수요와 공급이 만나 균형을 이루는 지점에서 결정돼요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>팬데믹 동안 반도체 가격이 상승한 주요 이유는 무엇인가요?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>반도체 공장 중단으로 공급이 감소하고, 원격 근무 확산으로 수요가 증가했기 때문이다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">팬데믹 동안 반도체 생산 공장이 중단되며 공급이 급격히 줄었고, 동시에 원격 근무와 온라인 교육 확산으로 노트북, 태블릿 등 전자기기의 수요가 급증했어요. 이로 인해 공급 곡선은 왼쪽으로, 수요 곡선은 오른쪽으로 이동하며 반도체 가격이 급등했죠. 공급 부족으로 자동차 제조사들은 생산량을 줄였고, 전자기기 가격은 상승했으며 대기 시간도 늘어났어요. 이 사례는 외부 요인이 수요와 공급 곡선을 이동시키고, 시장 가격과 거래량에 어떻게 영향을 미치는지 보여주는 대표적 예예요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 공급과 수요의 변화는 가격에 큰 영향을 미쳐요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>시장 가격</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>시장 가격은 수요와 공급이 균형을 이루는 지점에서 결정된다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">시장 가격은 소비자가 사고 싶어 하는 양(수요)과 생산자가 팔고 싶어 하는 양(공급)이 일치하는 지점에서 결정돼요. 예를 들어, 여름에 딸기가 많이 생산되면 공급이 증가하고, 이로 인해 딸기 가격이 내려가요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 시장 가격은 수요와 공급의 균형에서 형성돼요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>계절에 따라 딸기 가격이 변동하는 주요 원인은 무엇인가요?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공급 곡선 이동</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">딸기 가격은 계절에 따라 변동해요. 이는 딸기의 생산량, 즉 공급 곡선의 이동 때문이에요. 예를 들어, 겨울철 딸기가 많이 생산되면 공급 곡선이 오른쪽으로 이동하고 가격이 하락해요. 반대로 여름철 생산량이 줄면 공급 곡선이 왼쪽으로 이동하고 가격이 상승해요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 계절별 상품 가격 변화는 **공급 곡선 이동**과 관련돼요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>최저임금제가 노동 시장에서 실업을 초래할 수 있는 이유는 무엇인가요?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>고용주가 비용 부담을 느껴 노동 수요를 줄이기 때문이다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">최저임금제는 노동자의 기본 생활을 보장하기 위해 정부가 임금의 최저선을 설정하는 정책이에요. 하지만 최저임금이 균형 임금보다 높아지면 고용주는 비용 부담으로 노동 수요를 줄일 수 있어요. 결과적으로 노동 공급이 수요를 초과하며 실업이 발생할 수 있죠. 예를 들어, 한국에서 최저임금 인상 이후 일부 소상공인이 고용을 줄이고 무인 시스템을 도입한 사례가 있어요. 이는 최저임금이 소득 증대라는 긍정적 효과와 함께 고용 감소라는 부작용을 가져올 수 있음을 보여줘요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 정부의 가격 개입은 시장 균형을 왜곡할 수 있어요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기회 비용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기회비용은 선택하지 않은 옵션에서 얻을 수 있었던 가치를 의미한다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">기회비용은 어떤 선택을 할 때 포기한 다른 선택의 가치를 뜻해요. 예를 들어, 주말에 아르바이트 대신 친구와 여행을 갔다면, 아르바이트로 벌 수 있었던 돈이 기회비용이에요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 기회비용은 한정된 자원을 효율적으로 사용하는 데 도움을 줘요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기회비용은 어떤 선택을 할 때 포기한 다른 선택의 가치를 의미해요. 그렇다면, 기회비용과 가장 밀접하게 관련된 경제 개념은 무엇인가요?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>합리적 선택</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">기회비용은 선택의 대가로 포기하는 다른 기회의 가치를 뜻해요. 이는 제한된 자원을 효율적으로 사용하기 위한 **합리적 선택**과 밀접한 관련이 있어요. 예를 들어, 친구와 놀러 갈지 공부할지를 고민할 때, 두 선택의 기회비용을 비교하며 합리적인 결정을 내리게 돼요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 기회비용은 합리적인 의사결정을 내리기 위한 중요한 경제 개념이에요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>복지 예산 투자로 발생할 수 있는 주요 기회비용은 무엇인가요?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>도로 건설 지연으로 물류 비용이 증가할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">복지 예산 투자로 국민 건강과 삶의 질이 향상되며 의료비 절감 효과를 기대할 수 있어요. 하지만 복지 예산이 증가하면 도로 건설이나 물류 시스템 개선 같은 인프라 투자의 기회는 포기하게 돼요. 이는 물류 비용 증가와 경제 성장 둔화로 이어질 수 있죠. 예를 들어, 스웨덴은 복지 확대를 통해 사회 안정성을 강화했지만, 인프라 투자가 상대적으로 줄며 경제 성장 속도가 둔화됐어요. 국가 정책은 한정된 자원에서 어떤 선택이 장기적으로 더 유리한지를 신중히 고려해야 해요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 정책 결정에서도 기회비용은 중요한 고려 요소예요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>비용-수익 분석</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>비용-수익 분석은 선택의 비용과 수익을 비교하는 과정을 의미한다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">비용-수익 분석은 어떤 선택에 들어가는 비용과 그 선택으로 얻는 수익을 비교하는 과정이에요. 예를 들어, 편의점에서 도시락을 사는 경우, 도시락 가격과 이동 시간이 비용이고, 만족감이 수익이에요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 비용보다 수익이 크면 합리적인 선택이에요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>비용-수익 분석에서 선택의 간접 비용으로 고려해야 하는 요소는 무엇인가요?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기회비용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">비용-수익 분석은 직접 비용(예: 고정 비용, 변동 비용)과 간접 비용(예: 기회비용)을 모두 고려해야 해요. 간접 비용 중에서도 가장 중요한 것은 기회비용이에요. 예를 들어, 카페 창업을 위해 1억 원을 투자하면, 그 돈으로 다른 투자 기회를 놓친다는 점에서 기회비용이 발생해요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 비용-수익 분석에서는 눈에 보이는 직접 비용뿐만 아니라, 기회비용 같은 간접 비용도 꼭 고려해야 해요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>탄소 배출 규제 정책의 비용-수익 분석에서 장기적으로 기대되는 주요 수익은 무엇인가요?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>국민 건강 증진과 신재생 에너지 산업 활성화</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">탄소 배출 규제는 기업들에게 초기 시설 개선 비용과 기술 도입 부담을 요구해요. 하지만 장기적으로는 대기오염 감소로 국민 건강이 개선되고 의료비가 절감되는 효과가 있어요. 또한 신재생 에너지 산업이 성장하며 경제 발전과 신규 일자리 창출을 이끌어낼 수 있죠. 유럽연합은 초기의 큰 비용에도 불구하고 환경과 경제 모두에서 긍정적인 결과를 얻은 사례예요. 이 사례는 초기 비용보다 장기적 수익을 고려한 정책 설계와 비용-수익 분석의 중요성을 잘 보여줘요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> 핵심 정리: 초기 비용이 크더라도 장기적으로 큰 수익이 기대된다면 비용-수익 분석에서 긍정적인 결론을 내릴 수 있어요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>금융 기초</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>은행에 돈을 맡기면 이자를 받을 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>저축과 이자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">은행은 고객이 맡긴 돈(예금)을 다른 사람이나 기업에 대출해요. 이 과정에서 은행은 고객의 돈을 사용한 대가로 이자를 지급해요. 예를 들어, A씨가 100만 원을 연 3% 금리로 정기예금에 예치하면, 1년 후 이자로 3만 원을 추가로 받아 총 103만 원이 돼요. 저축은 자산을 늘리는 방법일 뿐만 아니라, 미래의 예상치 못한 상황에 대비하거나 목표를 달성하기 위한 필수적인 재무 전략이에요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 은행은 예금자를 통해 자금을 모으고, 이자를 지급하며 자산 증대를 도와요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>은행이 고객의 예금으로 대출을 제공하며 얻는 수익을 의미하는 경제 용어는 무엇인가요?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>금리 차이</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">은행은 예금자에게 이자를 지급하고, 대출자에게 이자를 받는 구조로 운영돼요. 예를 들어, 예금 금리가 연 3%이고, 대출 금리가 연 5%라면 은행은 5%-3%=2%의 금리 차이를 통해 수익을 창출해요. 이 금리 차이는 은행의 운영비용을 충당하고, 대출 리스크를 관리하며 이윤을 남기는 핵심 원천이에요. 금리 차이를 통해 금융 시스템은 원활히 작동하며, 은행은 자금을 효율적으로 순환시켜 경제를 활성화합니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 금리 차이는 은행의 주요 수익원이자 금융 시스템의 핵심 원리예요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>금리 인상이 경제에 미치는 영향을 가장 잘 설명한 것은 무엇인가요?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>금리가 인상되면 저축은 증가하고, 소비와 투자는 감소한다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">금리가 인상되면 예금 금리가 상승해 저축의 매력이 커져요. 반면, 대출 금리가 오르며 대출받은 자금에 대한 상환 부담이 증가하기 때문에 소비와 투자가 줄어들게 돼요. 예를 들어, 대출 금리가 2%에서 5%로 상승하면, 1억 원 대출 시 연 이자는 200만 원에서 500만 원으로 증가해요. 이는 기업과 개인이 투자를 축소하고, 소비를 줄이게 만들어 경제 성장 속도를 둔화시킬 수 있어요. 그러나 물가 상승 억제와 금융 안정성을 강화하는 데는 긍정적인 역할을 합니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 금리 인상은 저축 증가, 소비·투자 감소로 경제에 큰 영향을 미쳐요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>은행의 역할</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>은행은 사람들이 돈을 안전하게 보관하고 필요한 사람에게 빌려주는 중개자 역할을 한다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">은행은 개인과 기업의 돈을 안전하게 보관하는 동시에, 자금이 필요한 사람들에게 대출을 제공해요. 예를 들어, A씨가 저축한 돈을 통해 B씨가 대출을 받아 사업을 시작할 수 있어요. 이 과정에서 은행은 자금을 효율적으로 재분배하며, 금리 차이를 통해 운영비를 충당하고 경제 활동을 지원해요. 은행은 이러한 중개자 역할로 개인의 금융 안전망을 제공하고, 경제의 원활한 자금 흐름을 유지합니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 은행은 돈을 보관·대출하며 경제의 자금 흐름을 관리하는 중개자예요</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>은행이 고객의 자산을 효율적으로 운용하기 위해 제공하는 서비스는 무엇인가요?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 결제 서비스
+2. 신용 창출
+3. 자산 관리
+4. 대출 제공</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자산 관리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">은행은 정기예금, 적금, 펀드, 보험 등 다양한 금융 상품을 통해 고객이 자산을 안전하게 관리하고 증대할 수 있도록 지원해요. 예를 들어, C씨가 정기예금에 1천만 원을 예치하면, 안정적으로 이자를 받으며 자산을 불릴 수 있어요. 또한, 투자형 상품을 통해 장기적인 자산 증대도 기대할 수 있어요. 자산 관리는 개인의 재정 안정뿐만 아니라 경제 전반의 안정성에도 기여해요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 자산 관리는 은행의 금융 서비스 중 하나로, 고객의 자산 증대와 안정에 기여해요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2008년 글로벌 금융위기 당시 은행의 문제와 이를 해결하기 위한 대응을 가장 잘 설명한 것은 무엇인가요?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>은행의 부실 대출이 위기의 원인이었으며, 정부는 자금을 투입해 은행을 구제하고 금융 규제를 강화했다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 은행의 부실 대출이 증가했지만, 정부는 적극적으로 개입하지 않았다.
+2. 은행의 부실 대출이 위기의 원인이었으며, 정부는 자금을 투입해 은행을 구제하고 금융 규제를 강화했다.
+3. 금융위기는 은행과 무관하며, 대출 증가로 인해 발생했다.
+4. 정부는 금융위기 동안 금리를 대폭 인상해 소비와 투자를 촉진했다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2008년 금융위기는 은행의 부실 대출(서브프라임 모기지)로 시작됐어요. 위험한 대출 상품이 부동산 가격 하락과 함께 대규모 손실로 이어졌고, 은행은 파산 위기에 처했어요. 정부와 중앙은행은 대규모 구제 금융을 통해 은행에 자금을 공급했고, 금융 규제를 강화해 위기를 완화했어요. 예금자 보호 제도와 자본 비율 기준이 강화되며 금융 안정성을 회복했고, 이후 은행은 리스크 관리에 더 신중해졌어요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 2008년 금융위기는 은행 부실 대출에서 시작됐으며, 정부의 적극적 개입으로 해결됐어요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. O
+2. X</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 금리가 인상되면 저축은 감소하고, 대출은 증가한다.
+2. 금리가 인상되면 저축은 증가하고, 소비와 투자는 감소한다.
+3. 금리 인상은 경제 활동에 큰 영향을 미치지 않는다.
+4. 금리 인상은 물가 상승을 유발한다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 예금자 보호
+2. 금리 차이
+3. 기준 금리
+4. 금융 안정성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 기업의 초기 투자 부담 감소
+2. 대기오염 악화와 관련된 의료비 증가
+3. 국민 건강 증진과 신재생 에너지 산업 활성화
+4. 기업의 규제 시행 비용 절감</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 기회비용
+2. 고정 비용
+3. 변동 비용
+4. 한계 수익</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 국민 건강이 악화될 가능성이 높아진다.
+2. 도로 건설 지연으로 물류 비용이 증가할 수 있다.
+3. 신규 일자리 창출이 지나치게 많아질 수 있다.
+4. GDP 성장률이 지나치게 높아질 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 합리적 선택
+2. 한계 효용
+3. 한계 비용
+4. 공급 과잉</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 노동 공급이 감소하기 때문이다.
+2. 노동 수요가 증가하기 때문이다.
+3. 고용주가 비용 부담을 느껴 노동 수요를 줄이기 때문이다.
+4. 노동자가 최저임금 이상을 요구하기 때문이다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 공급 곡선 이동
+2. 한계 효용 체감
+3. 기회비용 증가
+4. 시장 독점</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 팬데믹으로 인해 반도체 수요가 감소했기 때문이다.
+2. 반도체 공장 중단으로 공급이 감소하고, 원격 근무 확산으로 수요가 증가했기 때문이다.
+3. 국제 경제 상황이 안정되면서 수요와 공급이 모두 감소했기 때문이다.
+4. 반도체 시장에 새로운 경쟁자가 등장했기 때문이다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 균형 가격
+2. 최저 가격
+3. 기회비용
+4. 한계 비용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>보통예금은 언제든지 돈을 인출할 수 있지만, 이자가 낮다.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">보통예금은 돈을 필요할 때 언제든 꺼낼 수 있어 편리하지만, 은행 입장에서는 장기적으로 활용하기 어려워 낮은 금리를 제공해요. 반면, 정기예금은 일정 기간 동안 인출하지 않도록 약정되어 더 높은 금리를 제공해요. 예를 들어, 보통예금 금리가 연 0.5%라면, 정기예금은 연 3%로 높은 금리를 받을 수 있어요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 보통예금은 편리성, 정기예금은 높은 이자를 제공해요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>예금을 기반으로 대출을 제공하며 경제 활동을 촉진하는 은행의 기능은 무엇인가요?</t>
+  </si>
+  <si>
+    <t>신용 창출</t>
+  </si>
+  <si>
+    <t>1. 신용 창출
+2. 결제 서비스
+3. 금융 규제
+4. 금리 관리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">은행은 고객의 예금을 활용해 대출을 제공하며, 이를 통해 신용을 창출하고 경제를 활성화해요. 예를 들어, A씨의 예금이 B씨의 대출 자금으로 사용돼, B씨가 공장을 짓고 경제 활동을 확장할 수 있어요. 이 과정에서 은행은 자금을 재분배하고, 개인과 기업의 금융 요구를 충족시켜 경제 성장을 촉진합니다.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 신용 창출은 은행이 자금을 재분배하며 경제 성장을 이끄는 핵심 기능이에요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기준금리 인하가 예금과 대출에 미치는 영향을 가장 잘 설명한 것은 무엇인가요?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 기준금리가 인하되면 예금 금리가 상승하고 대출 금리가 하락한다.
+2. 기준금리 인하는 예금과 대출 금리에 영향을 미치지 않는다.
+3. 기준금리가 인하되면 예금 금리가 하락하고 대출 금리가 하락해 소비와 투자가 증가한다.
+4. 기준금리 인하로 대출 금리가 상승해 기업의 투자 부담이 증가한다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기준금리가 인하되면 예금 금리가 하락하고 대출 금리가 하락해 소비와 투자가 증가한다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">기준금리는 시장 금리의 기준이 돼요. 기준금리가 인하되면 은행의 예금 금리와 대출 금리가 모두 하락해요. 이는 예금자에게는 저축의 매력을 줄이고, 대출자에게는 이자 부담을 줄여 소비와 투자를 촉진해요. 예를 들어, 기준금리가 5%에서 1%로 하락하면, 기업은 더 낮은 금리로 자금을 빌려 공장을 증설하거나 신규 사업을 시작할 수 있어요.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Apple Color Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> **핵심 정리**: 기준금리 인하는 소비와 투자를 촉진하며 경제를 활성화해요.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -932,6 +1677,57 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="맑은 고딕 (본문)"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="맑은 고딕 (본문)"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Apple Color Emoji"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -955,7 +1751,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -967,6 +1763,30 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1324,12 +2144,12 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1342,8 +2162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF907395-158E-DC4F-90EE-9B4F0A8AD405}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView topLeftCell="A18" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1359,307 +2179,307 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="139">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="291">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="234">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="101">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="253">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="234">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="120">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="291">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="329">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="177">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="367">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="329">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="158">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="329">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="272">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="215">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="234">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="272">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="291">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="234">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="234">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1670,273 +2490,594 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A53DA8-4004-F147-83E2-B833EA7F0E02}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
-    <col min="4" max="4" width="39.7109375" customWidth="1"/>
-    <col min="5" max="5" width="54.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="54.140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="6"/>
+    <col min="8" max="8" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="79">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="79">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="124">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="79">
+      <c r="A5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="C5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E5" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="79">
+      <c r="A6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C6" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="124">
+      <c r="A7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C7" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+    </row>
+    <row r="8" spans="1:8" ht="64">
+      <c r="A8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="H8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="79">
+      <c r="A9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="124">
+      <c r="A10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+      <c r="H10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="79">
+      <c r="A11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E11" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="94">
+      <c r="A12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="139">
+      <c r="A13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+      <c r="C13" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="124">
+      <c r="A14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
+      <c r="H14" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="109">
+      <c r="A15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="109">
+      <c r="A16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="109">
+      <c r="A17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="E17" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="124">
+      <c r="A18" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="124">
+      <c r="A19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
+      <c r="C19" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="94">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="H20" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="109">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="94">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
         <v>7</v>
       </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" t="s">
-        <v>49</v>
+      <c r="C22" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>